<commit_message>
fill out num chapters for all books
</commit_message>
<xml_diff>
--- a/ref/KJV Bible Info.xlsx
+++ b/ref/KJV Bible Info.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamd\Documents\GitHub\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B678FA56-5B56-49B3-A577-C25D1A1351CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8343F330-1978-4013-945A-348675616076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25860" yWindow="4980" windowWidth="5805" windowHeight="15510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
+    <sheet name="Chapters Count" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chapters!$A$1:$B$67</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Book</t>
   </si>
@@ -229,6 +233,12 @@
   </si>
   <si>
     <t>Revelation</t>
+  </si>
+  <si>
+    <t>Chapter</t>
+  </si>
+  <si>
+    <t>NumBooks</t>
   </si>
 </sst>
 </file>
@@ -252,12 +262,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -282,9 +298,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -566,17 +583,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -603,7 +621,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -627,7 +645,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -635,7 +653,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -643,7 +661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -651,7 +669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -659,7 +677,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -667,7 +685,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -675,7 +693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -683,7 +701,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -699,7 +717,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -707,7 +725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -715,7 +733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -739,7 +757,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -747,7 +765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -755,7 +773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -779,7 +797,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -795,7 +813,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -803,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -811,7 +829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -819,7 +837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -827,7 +845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -835,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -843,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -851,7 +869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -859,7 +877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -867,7 +885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -875,7 +893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -883,7 +901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -891,7 +909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -899,7 +917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -907,7 +925,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -915,7 +933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -923,7 +941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -931,7 +949,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -939,7 +957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -947,7 +965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -955,7 +973,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -963,7 +981,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -971,7 +989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -979,7 +997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -987,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -995,7 +1013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1003,7 +1021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1011,7 +1029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1019,7 +1037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1027,7 +1045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -1035,7 +1053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1043,7 +1061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1051,7 +1069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1059,7 +1077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1067,7 +1085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1075,7 +1093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1083,7 +1101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1091,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -1099,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1107,12 +1125,1247 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67">
         <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B67" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="greaterThan" val="33"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49B32A8-9917-41D6-A083-F346D1222EB2}">
+  <dimension ref="A1:B151"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed my first :bug: :praise: the Lord!
</commit_message>
<xml_diff>
--- a/ref/KJV Bible Info.xlsx
+++ b/ref/KJV Bible Info.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamd\Documents\GitHub\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8343F330-1978-4013-945A-348675616076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F99D1D-595E-4E09-BAB0-947A468F675D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25860" yWindow="4980" windowWidth="5805" windowHeight="15510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
     <sheet name="Chapters Count" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chapters!$A$1:$B$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chapters!$B$1:$C$67</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Book</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>NumBooks</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -583,564 +586,759 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>27</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>28</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>29</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>30</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>31</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>32</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>33</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>34</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>35</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>37</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>38</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>39</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>40</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>41</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>42</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>43</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>44</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
         <v>45</v>
       </c>
-      <c r="B45">
+      <c r="C45">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
         <v>46</v>
       </c>
-      <c r="B46">
+      <c r="C46">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>47</v>
       </c>
-      <c r="B47">
+      <c r="C47">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>48</v>
       </c>
-      <c r="B48">
+      <c r="C48">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
         <v>49</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
         <v>50</v>
       </c>
-      <c r="B50">
+      <c r="C50">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
         <v>51</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
         <v>52</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
         <v>53</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
         <v>54</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
         <v>55</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
         <v>56</v>
       </c>
-      <c r="B56">
+      <c r="C56">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
         <v>57</v>
       </c>
-      <c r="B57">
+      <c r="C57">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
         <v>58</v>
       </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
         <v>59</v>
       </c>
-      <c r="B59">
+      <c r="C59">
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
         <v>60</v>
       </c>
-      <c r="B60">
+      <c r="C60">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
         <v>61</v>
       </c>
-      <c r="B61">
+      <c r="C61">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
         <v>62</v>
       </c>
-      <c r="B62">
+      <c r="C62">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
         <v>63</v>
       </c>
-      <c r="B63">
+      <c r="C63">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
         <v>64</v>
       </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
         <v>65</v>
       </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
         <v>66</v>
       </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
         <v>67</v>
       </c>
-      <c r="B67">
+      <c r="C67">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B67" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="greaterThan" val="33"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:C67" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1149,9 +1347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49B32A8-9917-41D6-A083-F346D1222EB2}">
   <dimension ref="A1:B151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:B13"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix issues in chapters.json; Esther had too many chapters
</commit_message>
<xml_diff>
--- a/ref/KJV Bible Info.xlsx
+++ b/ref/KJV Bible Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamd\Documents\GitHub\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F99D1D-595E-4E09-BAB0-947A468F675D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5308AB-0CBB-44E0-8F8D-EA30073C1F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -274,7 +274,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,11 +586,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +689,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -765,7 +766,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -776,7 +777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -787,7 +788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -831,7 +832,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -842,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -875,7 +876,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -897,7 +898,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -908,7 +909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -919,7 +920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -930,7 +931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -941,7 +942,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -952,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -963,7 +964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -974,7 +975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -985,7 +986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -996,7 +997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1007,7 +1008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1018,7 +1019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1029,7 +1030,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1117,7 +1118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1128,7 +1129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1139,7 +1140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1150,7 +1151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1161,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1194,7 +1195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1205,7 +1206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1227,7 +1228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1249,7 +1250,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1260,7 +1261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1282,7 +1283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1293,7 +1294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1304,7 +1305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1315,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1338,7 +1339,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C67" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:C67" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="greaterThan" val="15"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1347,9 +1354,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49B32A8-9917-41D6-A083-F346D1222EB2}">
   <dimension ref="A1:B151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,90 +1374,90 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>34</v>
       </c>
     </row>
@@ -1463,146 +1470,146 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add script for querying verse count
</commit_message>
<xml_diff>
--- a/ref/KJV Bible Info.xlsx
+++ b/ref/KJV Bible Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamd\Documents\GitHub\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E31305-74D1-4E8E-87E3-8288C80E812F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0246551-4DAC-492E-939B-241E4837738D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -1026,6 +1026,92 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{242EF3D9-AF98-4768-AC7B-662D28C8172B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11115675" y="5772150"/>
+          <a:ext cx="3314700" cy="1190625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Notes</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>I</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> am unsure of the exact accuracy of this data as it came from a Catholic website.  Their Bible has extra books and verses compared to the KJV.  I have not checked all of these numbers manually.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4210,7 +4296,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12196,6 +12282,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix query to count verses not chapters
</commit_message>
<xml_diff>
--- a/ref/KJV Bible Info.xlsx
+++ b/ref/KJV Bible Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamd\Documents\GitHub\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0246551-4DAC-492E-939B-241E4837738D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3966B5-BA01-45A0-80DB-79F0D119CB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -950,7 +950,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -972,16 +972,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -998,20 +1011,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1032,16 +1064,96 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AD136F3-A5A5-49BF-9919-422A4029E49D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3124200" y="34194751"/>
+          <a:ext cx="3571875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> number matches this website: https://www.biblebelievers.com/believers-org/kjv-stats.html?_e_pi_=7%2CPAGE_ID10%2C1665113068</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1056,7 +1168,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11115675" y="5772150"/>
+          <a:off x="2476500" y="13344525"/>
           <a:ext cx="3314700" cy="1190625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1092,7 +1204,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100" u="sng"/>
             <a:t>Notes</a:t>
           </a:r>
         </a:p>
@@ -1103,7 +1215,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> am unsure of the exact accuracy of this data as it came from a Catholic website.  Their Bible has extra books and verses compared to the KJV.  I have not checked all of these numbers manually.</a:t>
+            <a:t> am unsure of the exact accuracy of this data as it came from a Catholic website.  Their Bible has extra books and verses compared to the KJV.  I have not checked all of these numbers manually.  Their total verse count is 167 verses over </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -1385,11 +1497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B67"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,6 +2248,12 @@
         <v>22</v>
       </c>
     </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="6">
+        <f>SUM(C2:C67)</f>
+        <v>1189</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C67">
@@ -2148,11 +2266,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49B32A8-9917-41D6-A083-F346D1222EB2}">
-  <dimension ref="A1:B151"/>
+  <dimension ref="A1:B152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3367,6 +3485,12 @@
       </c>
       <c r="B151">
         <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B152" s="6">
+        <f>SUM(B2:B151)</f>
+        <v>1189</v>
       </c>
     </row>
   </sheetData>
@@ -3381,11 +3505,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC86EBCD-116E-48E7-A257-C35B58BA5FDB}">
-  <dimension ref="A1:B177"/>
+  <dimension ref="A1:B178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J178" sqref="J178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3406,897 +3530,1432 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1189</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1189</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>1188</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>1184</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>1183</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>1174</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>1162</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>1152</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>1135</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>1118</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>1098</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>1075</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>1049</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>1012</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
+      </c>
+      <c r="B177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B178" s="6">
+        <f>SUM(B2:B177)</f>
+        <v>31102</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{FC86EBCD-116E-48E7-A257-C35B58BA5FDB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E697C1A6-2262-4EC1-8FB3-D0DD61AA811D}">
-  <dimension ref="A1:EW67"/>
+  <dimension ref="A1:EW68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R29" sqref="R29"/>
+      <selection pane="bottomRight" activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12277,6 +12936,12 @@
         <v>265</v>
       </c>
     </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C68" s="7">
+        <f>SUM(C2:C67)</f>
+        <v>31269</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:EW67" xr:uid="{E697C1A6-2262-4EC1-8FB3-D0DD61AA811D}"/>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
up to 2nd sam done
</commit_message>
<xml_diff>
--- a/ref/KJV Bible Info.xlsx
+++ b/ref/KJV Bible Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamd\Documents\GitHub\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0E17C5-8787-4BD0-AC54-28DF87390A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EB221A-3147-4974-B2EB-3EF46F8CFDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -1521,9 +1521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K61" sqref="K61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,101 +1545,101 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="8">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="8">
         <v>31</v>
       </c>
     </row>
@@ -2291,7 +2291,7 @@
   <dimension ref="A1:B152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
@@ -4977,11 +4977,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E697C1A6-2262-4EC1-8FB3-D0DD61AA811D}">
   <dimension ref="A1:EW68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4:AD4"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
finished first 20 books
</commit_message>
<xml_diff>
--- a/ref/KJV Bible Info.xlsx
+++ b/ref/KJV Bible Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamd\Documents\GitHub\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EB221A-3147-4974-B2EB-3EF46F8CFDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A971A30-5A81-42DD-A613-6739438F861C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1522,8 +1522,8 @@
   <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8:E8"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,123 +1644,123 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="8">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="8">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="8">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="8">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="8">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="8">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="8">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="8">
         <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="8">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
checked up to proverbs
</commit_message>
<xml_diff>
--- a/ref/KJV Bible Info.xlsx
+++ b/ref/KJV Bible Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamd\Documents\GitHub\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667BBD3D-301F-41ED-AFCF-10028EC42428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BD5380-5F6D-4FFD-8647-F8E0FA899492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -902,7 +902,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -912,6 +912,7 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1367,9 +1368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A35:C39"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,739 +1381,739 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="2">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="2">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="2">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="2">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="2">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="2">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="2">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="2">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="2">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="2">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="2">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="2">
         <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="2">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="2">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="2">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="2">
         <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
+      <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+      <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="2">
         <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="2">
         <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="2">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="2">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="2">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="2">
         <v>51</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="2">
         <v>52</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="2">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="2">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="2">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="2">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="2">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="2">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="2">
         <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="2">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="2">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="2">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="2">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="A64" s="2">
         <v>63</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="A65" s="2">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="A66" s="2">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="A67" s="2">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="2">
         <v>22</v>
       </c>
     </row>
@@ -4823,11 +4824,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E697C1A6-2262-4EC1-8FB3-D0DD61AA811D}">
   <dimension ref="A1:EW68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5791,119 +5792,119 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="0"/>
         <v>1288</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>54</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>34</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5">
         <v>51</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5">
         <v>49</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5">
         <v>31</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5">
         <v>27</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5">
         <v>89</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5">
         <v>26</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
         <v>23</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5">
         <v>36</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5">
         <v>35</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5">
         <v>16</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5">
         <v>33</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5">
         <v>45</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5">
         <v>41</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5">
+        <v>50</v>
+      </c>
+      <c r="T5">
+        <v>13</v>
+      </c>
+      <c r="U5">
+        <v>32</v>
+      </c>
+      <c r="V5">
+        <v>22</v>
+      </c>
+      <c r="W5">
+        <v>29</v>
+      </c>
+      <c r="X5">
         <v>35</v>
       </c>
-      <c r="T5" s="4">
-        <v>28</v>
-      </c>
-      <c r="U5" s="4">
-        <v>32</v>
-      </c>
-      <c r="V5" s="4">
-        <v>22</v>
-      </c>
-      <c r="W5" s="4">
+      <c r="Y5">
+        <v>41</v>
+      </c>
+      <c r="Z5">
+        <v>30</v>
+      </c>
+      <c r="AA5">
+        <v>25</v>
+      </c>
+      <c r="AB5">
+        <v>18</v>
+      </c>
+      <c r="AC5">
+        <v>65</v>
+      </c>
+      <c r="AD5">
+        <v>23</v>
+      </c>
+      <c r="AE5">
+        <v>31</v>
+      </c>
+      <c r="AF5">
+        <v>40</v>
+      </c>
+      <c r="AG5">
+        <v>16</v>
+      </c>
+      <c r="AH5">
+        <v>54</v>
+      </c>
+      <c r="AI5">
+        <v>42</v>
+      </c>
+      <c r="AJ5">
+        <v>56</v>
+      </c>
+      <c r="AK5">
         <v>29</v>
       </c>
-      <c r="X5" s="4">
-        <v>35</v>
-      </c>
-      <c r="Y5" s="4">
-        <v>41</v>
-      </c>
-      <c r="Z5" s="4">
-        <v>30</v>
-      </c>
-      <c r="AA5" s="4">
-        <v>25</v>
-      </c>
-      <c r="AB5" s="4">
-        <v>18</v>
-      </c>
-      <c r="AC5" s="4">
-        <v>65</v>
-      </c>
-      <c r="AD5" s="4">
-        <v>23</v>
-      </c>
-      <c r="AE5" s="4">
-        <v>31</v>
-      </c>
-      <c r="AF5" s="4">
-        <v>39</v>
-      </c>
-      <c r="AG5" s="4">
-        <v>17</v>
-      </c>
-      <c r="AH5" s="4">
-        <v>54</v>
-      </c>
-      <c r="AI5" s="4">
-        <v>42</v>
-      </c>
-      <c r="AJ5" s="4">
-        <v>56</v>
-      </c>
-      <c r="AK5" s="4">
-        <v>29</v>
-      </c>
-      <c r="AL5" s="4">
+      <c r="AL5">
         <v>34</v>
       </c>
-      <c r="AM5" s="4">
+      <c r="AM5">
         <v>13</v>
       </c>
       <c r="AN5" s="4" t="s">
@@ -5953,113 +5954,113 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
         <v>959</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>46</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>37</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
         <v>29</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6">
         <v>49</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <v>33</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <v>25</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6">
         <v>26</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6">
         <v>20</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6">
         <v>29</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6">
         <v>22</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6">
         <v>32</v>
       </c>
-      <c r="O6" s="4">
-        <v>31</v>
-      </c>
-      <c r="P6" s="4">
+      <c r="O6">
+        <v>32</v>
+      </c>
+      <c r="P6">
+        <v>18</v>
+      </c>
+      <c r="Q6">
+        <v>29</v>
+      </c>
+      <c r="R6">
+        <v>23</v>
+      </c>
+      <c r="S6">
+        <v>22</v>
+      </c>
+      <c r="T6">
+        <v>20</v>
+      </c>
+      <c r="U6">
+        <v>22</v>
+      </c>
+      <c r="V6">
+        <v>21</v>
+      </c>
+      <c r="W6">
+        <v>20</v>
+      </c>
+      <c r="X6">
+        <v>23</v>
+      </c>
+      <c r="Y6">
+        <v>30</v>
+      </c>
+      <c r="Z6">
+        <v>25</v>
+      </c>
+      <c r="AA6">
+        <v>22</v>
+      </c>
+      <c r="AB6">
         <v>19</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="AC6">
+        <v>19</v>
+      </c>
+      <c r="AD6">
+        <v>26</v>
+      </c>
+      <c r="AE6">
+        <v>68</v>
+      </c>
+      <c r="AF6">
         <v>29</v>
       </c>
-      <c r="R6" s="4">
-        <v>23</v>
-      </c>
-      <c r="S6" s="4">
-        <v>22</v>
-      </c>
-      <c r="T6" s="4">
+      <c r="AG6">
         <v>20</v>
       </c>
-      <c r="U6" s="4">
-        <v>22</v>
-      </c>
-      <c r="V6" s="4">
-        <v>21</v>
-      </c>
-      <c r="W6" s="4">
-        <v>20</v>
-      </c>
-      <c r="X6" s="4">
-        <v>23</v>
-      </c>
-      <c r="Y6" s="4">
+      <c r="AH6">
+        <v>30</v>
+      </c>
+      <c r="AI6">
+        <v>52</v>
+      </c>
+      <c r="AJ6">
         <v>29</v>
       </c>
-      <c r="Z6" s="4">
-        <v>26</v>
-      </c>
-      <c r="AA6" s="4">
-        <v>22</v>
-      </c>
-      <c r="AB6" s="4">
-        <v>19</v>
-      </c>
-      <c r="AC6" s="4">
-        <v>19</v>
-      </c>
-      <c r="AD6" s="4">
-        <v>26</v>
-      </c>
-      <c r="AE6" s="4">
-        <v>69</v>
-      </c>
-      <c r="AF6" s="4">
-        <v>28</v>
-      </c>
-      <c r="AG6" s="4">
-        <v>20</v>
-      </c>
-      <c r="AH6" s="4">
-        <v>30</v>
-      </c>
-      <c r="AI6" s="4">
-        <v>52</v>
-      </c>
-      <c r="AJ6" s="4">
-        <v>29</v>
-      </c>
-      <c r="AK6" s="4">
+      <c r="AK6">
         <v>12</v>
       </c>
       <c r="AL6" s="4" t="s">
@@ -6115,7 +6116,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="4">
@@ -6235,7 +6236,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4">
@@ -6355,7 +6356,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="4">
@@ -6475,7 +6476,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="4">
@@ -6543,19 +6544,19 @@
         <v>42</v>
       </c>
       <c r="X10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y10">
         <v>23</v>
       </c>
       <c r="Z10">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AA10">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB10">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AC10">
         <v>25</v>
@@ -6595,7 +6596,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="4">
@@ -6654,10 +6655,10 @@
         <v>29</v>
       </c>
       <c r="U11">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V11">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W11">
         <v>26</v>
@@ -6715,12 +6716,12 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D12">
         <v>53</v>
@@ -6732,10 +6733,10 @@
         <v>28</v>
       </c>
       <c r="G12">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H12">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="I12">
         <v>38</v>
@@ -6786,7 +6787,7 @@
         <v>29</v>
       </c>
       <c r="Y12">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Z12" t="s">
         <v>228</v>
@@ -6835,7 +6836,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="4">
@@ -6873,10 +6874,10 @@
         <v>36</v>
       </c>
       <c r="N13">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O13">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P13">
         <v>25</v>
@@ -6955,12 +6956,12 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D14">
         <v>54</v>
@@ -6975,10 +6976,10 @@
         <v>43</v>
       </c>
       <c r="H14">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="I14">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="J14">
         <v>40</v>
@@ -6996,7 +6997,7 @@
         <v>47</v>
       </c>
       <c r="O14">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P14">
         <v>14</v>
@@ -7075,18 +7076,18 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D15">
+        <v>17</v>
+      </c>
+      <c r="E15">
         <v>18</v>
-      </c>
-      <c r="E15">
-        <v>17</v>
       </c>
       <c r="F15">
         <v>17</v>
@@ -7119,10 +7120,10 @@
         <v>16</v>
       </c>
       <c r="P15">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R15">
         <v>19</v>
@@ -7185,7 +7186,7 @@
         <v>33</v>
       </c>
       <c r="AL15">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AM15">
         <v>23</v>
@@ -7195,7 +7196,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="4">
@@ -7315,12 +7316,12 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="0"/>
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D17">
         <v>11</v>
@@ -7329,10 +7330,10 @@
         <v>20</v>
       </c>
       <c r="F17">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G17">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H17">
         <v>19</v>
@@ -7341,16 +7342,16 @@
         <v>19</v>
       </c>
       <c r="J17">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K17">
         <v>18</v>
       </c>
       <c r="L17">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M17">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N17">
         <v>36</v>
@@ -7435,12 +7436,12 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="0"/>
-        <v>272</v>
+        <v>167</v>
       </c>
       <c r="D18">
         <v>22</v>
@@ -7472,24 +7473,12 @@
       <c r="M18">
         <v>3</v>
       </c>
-      <c r="N18">
-        <v>17</v>
-      </c>
-      <c r="O18">
-        <v>8</v>
-      </c>
-      <c r="P18">
-        <v>30</v>
-      </c>
-      <c r="Q18">
-        <v>16</v>
-      </c>
-      <c r="R18">
-        <v>24</v>
-      </c>
-      <c r="S18">
-        <v>10</v>
-      </c>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
       <c r="T18" t="s">
         <v>228</v>
       </c>
@@ -7555,12 +7544,12 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="0"/>
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="D19">
         <v>22</v>
@@ -7641,7 +7630,7 @@
         <v>14</v>
       </c>
       <c r="AD19">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AE19">
         <v>28</v>
@@ -7680,10 +7669,10 @@
         <v>30</v>
       </c>
       <c r="AQ19">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="AR19">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="AS19">
         <v>17</v>
@@ -7693,12 +7682,12 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="0"/>
-        <v>2526</v>
+        <v>2461</v>
       </c>
       <c r="D20">
         <v>6</v>
@@ -7707,25 +7696,25 @@
         <v>12</v>
       </c>
       <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>17</v>
+      </c>
+      <c r="K20">
         <v>9</v>
       </c>
-      <c r="G20">
-        <v>9</v>
-      </c>
-      <c r="H20">
-        <v>13</v>
-      </c>
-      <c r="I20">
-        <v>11</v>
-      </c>
-      <c r="J20">
-        <v>18</v>
-      </c>
-      <c r="K20">
-        <v>10</v>
-      </c>
       <c r="L20">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M20">
         <v>18</v>
@@ -7734,7 +7723,7 @@
         <v>7</v>
       </c>
       <c r="O20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P20">
         <v>6</v>
@@ -7752,19 +7741,19 @@
         <v>15</v>
       </c>
       <c r="U20">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V20">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y20">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z20">
         <v>6</v>
@@ -7776,7 +7765,7 @@
         <v>22</v>
       </c>
       <c r="AC20">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AD20">
         <v>14</v>
@@ -7788,10 +7777,10 @@
         <v>11</v>
       </c>
       <c r="AG20">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AH20">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AI20">
         <v>11</v>
@@ -7800,115 +7789,115 @@
         <v>22</v>
       </c>
       <c r="AK20">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AL20">
         <v>28</v>
       </c>
       <c r="AM20">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AN20">
         <v>40</v>
       </c>
       <c r="AO20">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AP20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AQ20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AR20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AS20">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AT20">
         <v>5</v>
       </c>
       <c r="AU20">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AV20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AW20">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AX20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AY20">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AZ20">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BA20">
         <v>23</v>
       </c>
       <c r="BB20">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="BC20">
+        <v>9</v>
+      </c>
+      <c r="BD20">
+        <v>6</v>
+      </c>
+      <c r="BE20">
+        <v>7</v>
+      </c>
+      <c r="BF20">
+        <v>23</v>
+      </c>
+      <c r="BG20">
+        <v>13</v>
+      </c>
+      <c r="BH20">
         <v>11</v>
       </c>
-      <c r="BD20">
-        <v>7</v>
-      </c>
-      <c r="BE20">
-        <v>9</v>
-      </c>
-      <c r="BF20">
-        <v>24</v>
-      </c>
-      <c r="BG20">
-        <v>14</v>
-      </c>
-      <c r="BH20">
+      <c r="BI20">
+        <v>11</v>
+      </c>
+      <c r="BJ20">
+        <v>17</v>
+      </c>
+      <c r="BK20">
         <v>12</v>
       </c>
-      <c r="BI20">
+      <c r="BL20">
+        <v>8</v>
+      </c>
+      <c r="BM20">
         <v>12</v>
       </c>
-      <c r="BJ20">
-        <v>18</v>
-      </c>
-      <c r="BK20">
-        <v>14</v>
-      </c>
-      <c r="BL20">
-        <v>9</v>
-      </c>
-      <c r="BM20">
+      <c r="BN20">
+        <v>11</v>
+      </c>
+      <c r="BO20">
+        <v>10</v>
+      </c>
+      <c r="BP20">
         <v>13</v>
-      </c>
-      <c r="BN20">
-        <v>12</v>
-      </c>
-      <c r="BO20">
-        <v>11</v>
-      </c>
-      <c r="BP20">
-        <v>14</v>
       </c>
       <c r="BQ20">
         <v>20</v>
       </c>
       <c r="BR20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BS20">
+        <v>35</v>
+      </c>
+      <c r="BT20">
         <v>36</v>
       </c>
-      <c r="BT20">
-        <v>37</v>
-      </c>
       <c r="BU20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="BV20">
         <v>24</v>
@@ -7923,13 +7912,13 @@
         <v>23</v>
       </c>
       <c r="BZ20">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="CA20">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="CB20">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="CC20">
         <v>72</v>
@@ -7938,22 +7927,22 @@
         <v>13</v>
       </c>
       <c r="CE20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="CF20">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="CG20">
         <v>8</v>
       </c>
       <c r="CH20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="CI20">
+        <v>12</v>
+      </c>
+      <c r="CJ20">
         <v>13</v>
-      </c>
-      <c r="CJ20">
-        <v>14</v>
       </c>
       <c r="CK20">
         <v>17</v>
@@ -7962,10 +7951,10 @@
         <v>7</v>
       </c>
       <c r="CM20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="CN20">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="CO20">
         <v>17</v>
@@ -7974,7 +7963,7 @@
         <v>16</v>
       </c>
       <c r="CQ20">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="CR20">
         <v>5</v>
@@ -8004,7 +7993,7 @@
         <v>8</v>
       </c>
       <c r="DA20">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="DB20">
         <v>22</v>
@@ -8022,7 +8011,7 @@
         <v>43</v>
       </c>
       <c r="DG20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="DH20">
         <v>31</v>
@@ -8118,13 +8107,13 @@
         <v>24</v>
       </c>
       <c r="EM20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="EN20">
         <v>10</v>
       </c>
       <c r="EO20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="EP20">
         <v>12</v>
@@ -8155,7 +8144,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="4">
@@ -12811,7 +12800,7 @@
     <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C68" s="6">
         <f>SUM(C2:C67)</f>
-        <v>31256</v>
+        <v>31088</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all books done; praise God!
</commit_message>
<xml_diff>
--- a/ref/KJV Bible Info.xlsx
+++ b/ref/KJV Bible Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamd\Documents\GitHub\personal_website\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802DE777-D78B-494E-8883-668DACFE3188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C792D916-30CD-471C-9A90-4F94EFD55CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -789,7 +789,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -819,15 +819,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -837,17 +830,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -884,13 +866,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -898,12 +879,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+  <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1283,13 +1261,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3276,11 +3254,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC86EBCD-116E-48E7-A257-C35B58BA5FDB}">
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:B178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3289,7 +3267,7 @@
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -3297,98 +3275,95 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="2">
         <v>1189</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="2">
         <v>1189</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="2">
         <v>1188</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="2">
         <v>1184</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="2">
         <v>1183</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="2">
         <v>1174</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
         <v>1162</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>1152</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
         <v>1135</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
         <v>1118</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
         <v>1098</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3396,7 +3371,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3404,7 +3379,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3412,7 +3387,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4726,11 +4701,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E697C1A6-2262-4EC1-8FB3-D0DD61AA811D}">
   <dimension ref="A1:EW68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomRight" activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10131,14 +10106,26 @@
       </c>
       <c r="C50" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
-      <c r="G50"/>
-      <c r="H50"/>
-      <c r="I50"/>
+        <v>155</v>
+      </c>
+      <c r="D50">
+        <v>23</v>
+      </c>
+      <c r="E50">
+        <v>22</v>
+      </c>
+      <c r="F50">
+        <v>21</v>
+      </c>
+      <c r="G50">
+        <v>32</v>
+      </c>
+      <c r="H50">
+        <v>33</v>
+      </c>
+      <c r="I50">
+        <v>24</v>
+      </c>
       <c r="J50"/>
       <c r="K50"/>
       <c r="L50"/>
@@ -10171,12 +10158,20 @@
       </c>
       <c r="C51" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D51"/>
-      <c r="E51"/>
-      <c r="F51"/>
-      <c r="G51"/>
+        <v>104</v>
+      </c>
+      <c r="D51">
+        <v>30</v>
+      </c>
+      <c r="E51">
+        <v>30</v>
+      </c>
+      <c r="F51">
+        <v>21</v>
+      </c>
+      <c r="G51">
+        <v>23</v>
+      </c>
       <c r="H51"/>
       <c r="I51"/>
       <c r="J51"/>
@@ -10211,12 +10206,20 @@
       </c>
       <c r="C52" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D52"/>
-      <c r="E52"/>
-      <c r="F52"/>
-      <c r="G52"/>
+        <v>95</v>
+      </c>
+      <c r="D52">
+        <v>29</v>
+      </c>
+      <c r="E52">
+        <v>23</v>
+      </c>
+      <c r="F52">
+        <v>25</v>
+      </c>
+      <c r="G52">
+        <v>18</v>
+      </c>
       <c r="H52"/>
       <c r="I52"/>
       <c r="J52"/>
@@ -10251,13 +10254,23 @@
       </c>
       <c r="C53" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D53"/>
-      <c r="E53"/>
-      <c r="F53"/>
-      <c r="G53"/>
-      <c r="H53"/>
+        <v>89</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>20</v>
+      </c>
+      <c r="F53">
+        <v>13</v>
+      </c>
+      <c r="G53">
+        <v>18</v>
+      </c>
+      <c r="H53">
+        <v>28</v>
+      </c>
       <c r="I53"/>
       <c r="J53"/>
       <c r="K53"/>
@@ -10291,11 +10304,17 @@
       </c>
       <c r="C54" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D54"/>
-      <c r="E54"/>
-      <c r="F54"/>
+        <v>47</v>
+      </c>
+      <c r="D54">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>17</v>
+      </c>
+      <c r="F54">
+        <v>18</v>
+      </c>
       <c r="G54"/>
       <c r="H54"/>
       <c r="I54"/>
@@ -10331,14 +10350,26 @@
       </c>
       <c r="C55" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
+        <v>113</v>
+      </c>
+      <c r="D55">
+        <v>20</v>
+      </c>
+      <c r="E55">
+        <v>15</v>
+      </c>
+      <c r="F55">
+        <v>16</v>
+      </c>
+      <c r="G55">
+        <v>16</v>
+      </c>
+      <c r="H55">
+        <v>25</v>
+      </c>
+      <c r="I55">
+        <v>21</v>
+      </c>
       <c r="J55"/>
       <c r="K55"/>
       <c r="L55"/>
@@ -10371,12 +10402,20 @@
       </c>
       <c r="C56" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D56"/>
-      <c r="E56"/>
-      <c r="F56"/>
-      <c r="G56"/>
+        <v>83</v>
+      </c>
+      <c r="D56">
+        <v>18</v>
+      </c>
+      <c r="E56">
+        <v>26</v>
+      </c>
+      <c r="F56">
+        <v>17</v>
+      </c>
+      <c r="G56">
+        <v>22</v>
+      </c>
       <c r="H56"/>
       <c r="I56"/>
       <c r="J56"/>
@@ -10411,11 +10450,17 @@
       </c>
       <c r="C57" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
+        <v>46</v>
+      </c>
+      <c r="D57">
+        <v>16</v>
+      </c>
+      <c r="E57">
+        <v>15</v>
+      </c>
+      <c r="F57">
+        <v>15</v>
+      </c>
       <c r="G57"/>
       <c r="H57"/>
       <c r="I57"/>
@@ -10451,9 +10496,11 @@
       </c>
       <c r="C58" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D58"/>
+        <v>25</v>
+      </c>
+      <c r="D58">
+        <v>25</v>
+      </c>
       <c r="E58"/>
       <c r="F58"/>
       <c r="G58"/>
@@ -10491,21 +10538,47 @@
       </c>
       <c r="C59" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D59"/>
-      <c r="E59"/>
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
-      <c r="J59"/>
-      <c r="K59"/>
-      <c r="L59"/>
-      <c r="M59"/>
-      <c r="N59"/>
-      <c r="O59"/>
-      <c r="P59"/>
+        <v>303</v>
+      </c>
+      <c r="D59">
+        <v>14</v>
+      </c>
+      <c r="E59">
+        <v>18</v>
+      </c>
+      <c r="F59">
+        <v>19</v>
+      </c>
+      <c r="G59">
+        <v>16</v>
+      </c>
+      <c r="H59">
+        <v>14</v>
+      </c>
+      <c r="I59">
+        <v>20</v>
+      </c>
+      <c r="J59">
+        <v>28</v>
+      </c>
+      <c r="K59">
+        <v>13</v>
+      </c>
+      <c r="L59">
+        <v>28</v>
+      </c>
+      <c r="M59">
+        <v>39</v>
+      </c>
+      <c r="N59">
+        <v>40</v>
+      </c>
+      <c r="O59">
+        <v>29</v>
+      </c>
+      <c r="P59">
+        <v>25</v>
+      </c>
       <c r="Q59"/>
       <c r="R59"/>
       <c r="S59"/>
@@ -10531,13 +10604,23 @@
       </c>
       <c r="C60" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
+        <v>108</v>
+      </c>
+      <c r="D60">
+        <v>27</v>
+      </c>
+      <c r="E60">
+        <v>26</v>
+      </c>
+      <c r="F60">
+        <v>18</v>
+      </c>
+      <c r="G60">
+        <v>17</v>
+      </c>
+      <c r="H60">
+        <v>20</v>
+      </c>
       <c r="I60"/>
       <c r="J60"/>
       <c r="K60"/>
@@ -10571,13 +10654,23 @@
       </c>
       <c r="C61" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
+        <v>105</v>
+      </c>
+      <c r="D61">
+        <v>25</v>
+      </c>
+      <c r="E61">
+        <v>25</v>
+      </c>
+      <c r="F61">
+        <v>22</v>
+      </c>
+      <c r="G61">
+        <v>19</v>
+      </c>
+      <c r="H61">
+        <v>14</v>
+      </c>
       <c r="I61"/>
       <c r="J61"/>
       <c r="K61"/>
@@ -10611,11 +10704,17 @@
       </c>
       <c r="C62" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
+        <v>61</v>
+      </c>
+      <c r="D62">
+        <v>21</v>
+      </c>
+      <c r="E62">
+        <v>22</v>
+      </c>
+      <c r="F62">
+        <v>18</v>
+      </c>
       <c r="G62"/>
       <c r="H62"/>
       <c r="I62"/>
@@ -10651,13 +10750,23 @@
       </c>
       <c r="C63" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
+        <v>105</v>
+      </c>
+      <c r="D63">
+        <v>10</v>
+      </c>
+      <c r="E63">
+        <v>29</v>
+      </c>
+      <c r="F63">
+        <v>24</v>
+      </c>
+      <c r="G63">
+        <v>21</v>
+      </c>
+      <c r="H63">
+        <v>21</v>
+      </c>
       <c r="I63"/>
       <c r="J63"/>
       <c r="K63"/>
@@ -10691,9 +10800,11 @@
       </c>
       <c r="C64" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D64"/>
+        <v>13</v>
+      </c>
+      <c r="D64">
+        <v>13</v>
+      </c>
       <c r="E64"/>
       <c r="F64"/>
       <c r="G64"/>
@@ -10731,9 +10842,11 @@
       </c>
       <c r="C65" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D65"/>
+        <v>14</v>
+      </c>
+      <c r="D65">
+        <v>14</v>
+      </c>
       <c r="E65"/>
       <c r="F65"/>
       <c r="G65"/>
@@ -10771,9 +10884,11 @@
       </c>
       <c r="C66" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D66"/>
+        <v>25</v>
+      </c>
+      <c r="D66">
+        <v>25</v>
+      </c>
       <c r="E66"/>
       <c r="F66"/>
       <c r="G66"/>
@@ -10811,30 +10926,74 @@
       </c>
       <c r="C67" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D67"/>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
-      <c r="I67"/>
-      <c r="J67"/>
-      <c r="K67"/>
-      <c r="L67"/>
-      <c r="M67"/>
-      <c r="N67"/>
-      <c r="O67"/>
-      <c r="P67"/>
-      <c r="Q67"/>
-      <c r="R67"/>
-      <c r="S67"/>
-      <c r="T67"/>
-      <c r="U67"/>
-      <c r="V67"/>
-      <c r="W67"/>
-      <c r="X67"/>
-      <c r="Y67"/>
+        <v>404</v>
+      </c>
+      <c r="D67">
+        <v>20</v>
+      </c>
+      <c r="E67">
+        <v>29</v>
+      </c>
+      <c r="F67">
+        <v>22</v>
+      </c>
+      <c r="G67">
+        <v>11</v>
+      </c>
+      <c r="H67">
+        <v>14</v>
+      </c>
+      <c r="I67">
+        <v>17</v>
+      </c>
+      <c r="J67">
+        <v>17</v>
+      </c>
+      <c r="K67">
+        <v>13</v>
+      </c>
+      <c r="L67">
+        <v>21</v>
+      </c>
+      <c r="M67">
+        <v>11</v>
+      </c>
+      <c r="N67">
+        <v>19</v>
+      </c>
+      <c r="O67">
+        <v>17</v>
+      </c>
+      <c r="P67">
+        <v>18</v>
+      </c>
+      <c r="Q67">
+        <v>20</v>
+      </c>
+      <c r="R67">
+        <v>8</v>
+      </c>
+      <c r="S67">
+        <v>21</v>
+      </c>
+      <c r="T67">
+        <v>18</v>
+      </c>
+      <c r="U67">
+        <v>24</v>
+      </c>
+      <c r="V67">
+        <v>21</v>
+      </c>
+      <c r="W67">
+        <v>15</v>
+      </c>
+      <c r="X67">
+        <v>27</v>
+      </c>
+      <c r="Y67">
+        <v>21</v>
+      </c>
       <c r="Z67"/>
       <c r="AA67"/>
       <c r="AB67"/>
@@ -10845,7 +11004,7 @@
     <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C68" s="6">
         <f>SUM(C2:C67)</f>
-        <v>29194</v>
+        <v>31089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>